<commit_message>
Massa de dados para cadastro de usuário
</commit_message>
<xml_diff>
--- a/HubTalentos-Avaliacao/AdvantageOnline_DataPageRegister.xlsx
+++ b/HubTalentos-Avaliacao/AdvantageOnline_DataPageRegister.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex.junior\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex.junior\Git\HubTalentosAvaliacao\HubTalentos-Avaliacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{360A08B4-6D0E-42F2-BAF9-C6DE1F39C06E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B04B0EC-26E0-47D9-B106-2288E15FAB54}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8D0779E8-EFC8-4813-BF37-B00537C68B16}"/>
   </bookViews>
@@ -290,9 +290,6 @@
     <t>1º</t>
   </si>
   <si>
-    <t>BRUNO345</t>
-  </si>
-  <si>
     <t>brunomarcos@teste.com</t>
   </si>
   <si>
@@ -321,6 +318,9 @@
   </si>
   <si>
     <t>5200 444</t>
+  </si>
+  <si>
+    <t>BRUNO370</t>
   </si>
 </sst>
 </file>
@@ -757,7 +757,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,37 +819,37 @@
         <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adicionada mais linhas de teste para a massa de dados
</commit_message>
<xml_diff>
--- a/HubTalentos-Avaliacao/AdvantageOnline_DataPageRegister.xlsx
+++ b/HubTalentos-Avaliacao/AdvantageOnline_DataPageRegister.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex.junior\Git\HubTalentosAvaliacao\HubTalentos-Avaliacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B04B0EC-26E0-47D9-B106-2288E15FAB54}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D154B0-754A-4913-B47A-1E83135EBC72}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8D0779E8-EFC8-4813-BF37-B00537C68B16}"/>
   </bookViews>
@@ -249,7 +249,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>NUMBER TEST</t>
   </si>
@@ -320,7 +320,79 @@
     <t>5200 444</t>
   </si>
   <si>
-    <t>BRUNO370</t>
+    <t>BRUNO383</t>
+  </si>
+  <si>
+    <t>2º</t>
+  </si>
+  <si>
+    <t>3º</t>
+  </si>
+  <si>
+    <t>Marcela</t>
+  </si>
+  <si>
+    <t>Matos</t>
+  </si>
+  <si>
+    <t>marcelamatos@teste.com</t>
+  </si>
+  <si>
+    <t>Marcela74</t>
+  </si>
+  <si>
+    <t>BrUn-^:1SW</t>
+  </si>
+  <si>
+    <t>blumenal@teste.com</t>
+  </si>
+  <si>
+    <t>Marcela.1234</t>
+  </si>
+  <si>
+    <t>paçoca123A</t>
+  </si>
+  <si>
+    <t>Blumenal</t>
+  </si>
+  <si>
+    <t>Souza</t>
+  </si>
+  <si>
+    <t>55 11 8542 3671</t>
+  </si>
+  <si>
+    <t>57 21 8545 3535</t>
+  </si>
+  <si>
+    <t>Bahamas</t>
+  </si>
+  <si>
+    <t>French Polynesia</t>
+  </si>
+  <si>
+    <t>Galapz</t>
+  </si>
+  <si>
+    <t>Martito</t>
+  </si>
+  <si>
+    <t>Futton Six</t>
+  </si>
+  <si>
+    <t>Street Max</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>LS</t>
+  </si>
+  <si>
+    <t>00 555 111 3</t>
+  </si>
+  <si>
+    <t>40852 41</t>
   </si>
 </sst>
 </file>
@@ -754,10 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA74D7E8-6402-4590-A29D-1B9CE9F8EE2E}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,12 +924,90 @@
         <v>22</v>
       </c>
     </row>
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{506B5F6E-04B9-42F4-B212-FF15B9BD919A}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{F17133B7-2C6B-415C-9D6B-D05BC20E0D31}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{2D786DDF-5728-4B60-AD28-AF599AF8C51C}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mais dados para a massa
</commit_message>
<xml_diff>
--- a/HubTalentos-Avaliacao/AdvantageOnline_DataPageRegister.xlsx
+++ b/HubTalentos-Avaliacao/AdvantageOnline_DataPageRegister.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex.junior\Git\HubTalentosAvaliacao\HubTalentos-Avaliacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D154B0-754A-4913-B47A-1E83135EBC72}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B7EC1F-B6C3-40EA-A258-C8DF360EACE8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8D0779E8-EFC8-4813-BF37-B00537C68B16}"/>
   </bookViews>
@@ -392,7 +392,7 @@
     <t>00 555 111 3</t>
   </si>
   <si>
-    <t>40852 41</t>
+    <t>40852 412</t>
   </si>
 </sst>
 </file>

</xml_diff>